<commit_message>
url factory retain url allready generated
</commit_message>
<xml_diff>
--- a/tools/visual-testing/workdir/source-files/example.xlsx
+++ b/tools/visual-testing/workdir/source-files/example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="24240" windowHeight="13740" activeTab="4"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="24240" windowHeight="13740" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="batnet" sheetId="2" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="97">
   <si>
     <t>Site comparaison</t>
   </si>
@@ -273,13 +273,50 @@
   </si>
   <si>
     <t>97%</t>
+  </si>
+  <si>
+    <t>21/01/2016 09:48</t>
+  </si>
+  <si>
+    <t>21/01/2016 09:49</t>
+  </si>
+  <si>
+    <t>21/01/2016 09:51</t>
+  </si>
+  <si>
+    <t>55%</t>
+  </si>
+  <si>
+    <t>99%</t>
+  </si>
+  <si>
+    <t>94%</t>
+  </si>
+  <si>
+    <t>72%</t>
+  </si>
+  <si>
+    <t>98%</t>
+  </si>
+  <si>
+    <t>83%</t>
+  </si>
+  <si>
+    <t>87%</t>
+  </si>
+  <si>
+    <t>96%</t>
+  </si>
+  <si>
+    <t>82%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -634,8 +671,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="58.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="58.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -663,7 +700,7 @@
         <v>71</v>
       </c>
       <c r="D2" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -685,7 +722,7 @@
         <v>72</v>
       </c>
       <c r="D4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -749,7 +786,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="68.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="68.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -777,7 +814,7 @@
         <v>71</v>
       </c>
       <c r="D2" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -932,7 +969,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="68.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="68.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -960,7 +997,7 @@
         <v>71</v>
       </c>
       <c r="D2" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1038,7 +1075,7 @@
         <v>73</v>
       </c>
       <c r="D8" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1126,18 +1163,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="68.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="68.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1150,8 +1187,11 @@
       <c r="D1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1164,8 +1204,11 @@
       <c r="D2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1173,7 +1216,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
@@ -1186,8 +1229,11 @@
       <c r="D4" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>24</v>
       </c>
@@ -1200,8 +1246,11 @@
       <c r="D5" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>25</v>
       </c>
@@ -1214,8 +1263,11 @@
       <c r="D6" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>30</v>
       </c>
@@ -1228,8 +1280,11 @@
       <c r="D7" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1242,8 +1297,11 @@
       <c r="D8" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1256,8 +1314,11 @@
       <c r="D9" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1270,8 +1331,11 @@
       <c r="D10" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -1283,6 +1347,9 @@
       </c>
       <c r="D11" t="s">
         <v>82</v>
+      </c>
+      <c r="E11" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1299,13 +1366,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="57.140625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="57.140625" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1332,6 +1399,9 @@
       <c r="C2" t="s">
         <v>83</v>
       </c>
+      <c r="D2" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -1351,6 +1421,9 @@
       <c r="C4" t="s">
         <v>72</v>
       </c>
+      <c r="D4" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1362,6 +1435,9 @@
       <c r="C5" t="s">
         <v>72</v>
       </c>
+      <c r="D5" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1373,6 +1449,9 @@
       <c r="C6" t="s">
         <v>84</v>
       </c>
+      <c r="D6" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1384,6 +1463,9 @@
       <c r="C7" t="s">
         <v>72</v>
       </c>
+      <c r="D7" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -1395,6 +1477,9 @@
       <c r="C8" t="s">
         <v>72</v>
       </c>
+      <c r="D8" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1406,6 +1491,9 @@
       <c r="C9" t="s">
         <v>72</v>
       </c>
+      <c r="D9" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1417,6 +1505,9 @@
       <c r="C10" t="s">
         <v>72</v>
       </c>
+      <c r="D10" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1428,6 +1519,9 @@
       <c r="C11" t="s">
         <v>72</v>
       </c>
+      <c r="D11" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1439,6 +1533,9 @@
       <c r="C12" t="s">
         <v>72</v>
       </c>
+      <c r="D12" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1450,6 +1547,9 @@
       <c r="C13" t="s">
         <v>72</v>
       </c>
+      <c r="D13" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1461,6 +1561,9 @@
       <c r="C14" t="s">
         <v>72</v>
       </c>
+      <c r="D14" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1472,6 +1575,9 @@
       <c r="C15" t="s">
         <v>72</v>
       </c>
+      <c r="D15" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1483,6 +1589,9 @@
       <c r="C16" t="s">
         <v>72</v>
       </c>
+      <c r="D16" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -1494,6 +1603,9 @@
       <c r="C17" t="s">
         <v>72</v>
       </c>
+      <c r="D17" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -1505,6 +1617,9 @@
       <c r="C18" t="s">
         <v>72</v>
       </c>
+      <c r="D18" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -1516,6 +1631,9 @@
       <c r="C19" t="s">
         <v>72</v>
       </c>
+      <c r="D19" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -1527,6 +1645,9 @@
       <c r="C20" t="s">
         <v>72</v>
       </c>
+      <c r="D20" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -1538,6 +1659,9 @@
       <c r="C21" t="s">
         <v>72</v>
       </c>
+      <c r="D21" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -1549,6 +1673,9 @@
       <c r="C22" t="s">
         <v>72</v>
       </c>
+      <c r="D22" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -1560,6 +1687,9 @@
       <c r="C23" t="s">
         <v>72</v>
       </c>
+      <c r="D23" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -1571,6 +1701,9 @@
       <c r="C24" t="s">
         <v>72</v>
       </c>
+      <c r="D24" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
@@ -1582,6 +1715,9 @@
       <c r="C25" t="s">
         <v>72</v>
       </c>
+      <c r="D25" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
@@ -1593,6 +1729,9 @@
       <c r="C26" t="s">
         <v>72</v>
       </c>
+      <c r="D26" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -1604,6 +1743,9 @@
       <c r="C27" t="s">
         <v>72</v>
       </c>
+      <c r="D27" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -1615,6 +1757,9 @@
       <c r="C28" t="s">
         <v>72</v>
       </c>
+      <c r="D28" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -1626,6 +1771,9 @@
       <c r="C29" t="s">
         <v>72</v>
       </c>
+      <c r="D29" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
@@ -1637,6 +1785,9 @@
       <c r="C30" t="s">
         <v>72</v>
       </c>
+      <c r="D30" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
@@ -1648,6 +1799,9 @@
       <c r="C31" t="s">
         <v>72</v>
       </c>
+      <c r="D31" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -1658,6 +1812,9 @@
       </c>
       <c r="C32" t="s">
         <v>72</v>
+      </c>
+      <c r="D32" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
date formated in info bean
</commit_message>
<xml_diff>
--- a/tools/visual-testing/workdir/source-files/example.xlsx
+++ b/tools/visual-testing/workdir/source-files/example.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="30" windowWidth="24240" windowHeight="13740" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="24240" windowHeight="13740" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="batnet" sheetId="2" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="divers" sheetId="4" r:id="rId3"/>
     <sheet name="atart" sheetId="5" r:id="rId4"/>
     <sheet name="BIs" sheetId="6" r:id="rId5"/>
+    <sheet name="fuorimondo" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="126">
   <si>
     <t>Site comparaison</t>
   </si>
@@ -257,58 +258,145 @@
     <t>comp3</t>
   </si>
   <si>
-    <t>20/01/2016 16:43</t>
+    <t>20/01/2016 16:44</t>
+  </si>
+  <si>
+    <t>51%</t>
+  </si>
+  <si>
+    <t>20/01/2016 16:45</t>
+  </si>
+  <si>
+    <t>97%</t>
+  </si>
+  <si>
+    <t>21/01/2016 09:48</t>
+  </si>
+  <si>
+    <t>21/01/2016 09:49</t>
+  </si>
+  <si>
+    <t>21/01/2016 09:51</t>
+  </si>
+  <si>
+    <t>55%</t>
+  </si>
+  <si>
+    <t>99%</t>
+  </si>
+  <si>
+    <t>94%</t>
+  </si>
+  <si>
+    <t>72%</t>
+  </si>
+  <si>
+    <t>98%</t>
+  </si>
+  <si>
+    <t>83%</t>
+  </si>
+  <si>
+    <t>87%</t>
+  </si>
+  <si>
+    <t>96%</t>
+  </si>
+  <si>
+    <t>82%</t>
+  </si>
+  <si>
+    <t>http://www.fuorimondo.com/fr/legend.html</t>
+  </si>
+  <si>
+    <t>http://www.fuorimondo.com/fr/location.html</t>
+  </si>
+  <si>
+    <t>http://www.fuorimondo.com/fr/network.html</t>
+  </si>
+  <si>
+    <t>http://www.fuorimondo.com/fr/media.html</t>
+  </si>
+  <si>
+    <t>http://www.fuorimondo.com/fr/vineyard/lino.html</t>
+  </si>
+  <si>
+    <t>10/02/2016 10:57</t>
+  </si>
+  <si>
+    <t>68%</t>
+  </si>
+  <si>
+    <t>45%</t>
+  </si>
+  <si>
+    <t>62%</t>
+  </si>
+  <si>
+    <t>64%</t>
+  </si>
+  <si>
+    <t>10/02/2016 10:58</t>
+  </si>
+  <si>
+    <t>46%</t>
+  </si>
+  <si>
+    <t>56%</t>
+  </si>
+  <si>
+    <t>57%</t>
+  </si>
+  <si>
+    <t>88%</t>
+  </si>
+  <si>
+    <t>89%</t>
+  </si>
+  <si>
+    <t>75%</t>
+  </si>
+  <si>
+    <t>10/02/2016 10:59</t>
+  </si>
+  <si>
+    <t>76%</t>
+  </si>
+  <si>
+    <t>67%</t>
+  </si>
+  <si>
+    <t>77%</t>
+  </si>
+  <si>
+    <t>70%</t>
+  </si>
+  <si>
+    <t>79%</t>
   </si>
   <si>
     <t>90%</t>
   </si>
   <si>
-    <t>20/01/2016 16:44</t>
-  </si>
-  <si>
-    <t>51%</t>
-  </si>
-  <si>
-    <t>20/01/2016 16:45</t>
-  </si>
-  <si>
-    <t>97%</t>
-  </si>
-  <si>
-    <t>21/01/2016 09:48</t>
-  </si>
-  <si>
-    <t>21/01/2016 09:49</t>
-  </si>
-  <si>
-    <t>21/01/2016 09:51</t>
-  </si>
-  <si>
-    <t>55%</t>
-  </si>
-  <si>
-    <t>99%</t>
-  </si>
-  <si>
-    <t>94%</t>
-  </si>
-  <si>
-    <t>72%</t>
-  </si>
-  <si>
-    <t>98%</t>
-  </si>
-  <si>
-    <t>83%</t>
-  </si>
-  <si>
-    <t>87%</t>
-  </si>
-  <si>
-    <t>96%</t>
-  </si>
-  <si>
-    <t>82%</t>
+    <t>59%</t>
+  </si>
+  <si>
+    <t>63%</t>
+  </si>
+  <si>
+    <t>93%</t>
+  </si>
+  <si>
+    <t>81%</t>
+  </si>
+  <si>
+    <t>91%</t>
+  </si>
+  <si>
+    <t>65%</t>
+  </si>
+  <si>
+    <t>10/02/2016 11:02</t>
   </si>
 </sst>
 </file>
@@ -700,7 +788,7 @@
         <v>71</v>
       </c>
       <c r="D2" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -722,7 +810,7 @@
         <v>72</v>
       </c>
       <c r="D4" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -736,7 +824,7 @@
         <v>72</v>
       </c>
       <c r="D5" t="s">
-        <v>72</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -750,7 +838,7 @@
         <v>72</v>
       </c>
       <c r="D6" t="s">
-        <v>72</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -764,7 +852,7 @@
         <v>72</v>
       </c>
       <c r="D7" t="s">
-        <v>72</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -814,7 +902,7 @@
         <v>71</v>
       </c>
       <c r="D2" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -836,7 +924,7 @@
         <v>72</v>
       </c>
       <c r="D4" t="s">
-        <v>72</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -906,7 +994,7 @@
         <v>72</v>
       </c>
       <c r="D9" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -997,7 +1085,7 @@
         <v>71</v>
       </c>
       <c r="D2" t="s">
-        <v>86</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1033,7 +1121,7 @@
         <v>72</v>
       </c>
       <c r="D5" t="s">
-        <v>72</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1047,7 +1135,7 @@
         <v>74</v>
       </c>
       <c r="D6" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1061,7 +1149,7 @@
         <v>72</v>
       </c>
       <c r="D7" t="s">
-        <v>72</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1075,7 +1163,7 @@
         <v>73</v>
       </c>
       <c r="D8" t="s">
-        <v>76</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1165,7 +1253,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -1202,10 +1290,10 @@
         <v>75</v>
       </c>
       <c r="D2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E2" t="s">
-        <v>87</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1230,7 +1318,7 @@
         <v>72</v>
       </c>
       <c r="E4" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1247,7 +1335,7 @@
         <v>72</v>
       </c>
       <c r="E5" t="s">
-        <v>72</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1264,7 +1352,7 @@
         <v>72</v>
       </c>
       <c r="E6" t="s">
-        <v>72</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1281,7 +1369,7 @@
         <v>72</v>
       </c>
       <c r="E7" t="s">
-        <v>72</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1298,7 +1386,7 @@
         <v>72</v>
       </c>
       <c r="E8" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1315,7 +1403,7 @@
         <v>72</v>
       </c>
       <c r="E9" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1332,7 +1420,7 @@
         <v>72</v>
       </c>
       <c r="E10" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1346,10 +1434,10 @@
         <v>76</v>
       </c>
       <c r="D11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E11" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1397,10 +1485,10 @@
         <v>77</v>
       </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D2" t="s">
-        <v>87</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1422,7 +1510,7 @@
         <v>72</v>
       </c>
       <c r="D4" t="s">
-        <v>90</v>
+        <v>121</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1436,7 +1524,7 @@
         <v>72</v>
       </c>
       <c r="D5" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1447,10 +1535,10 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D6" t="s">
-        <v>84</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1464,7 +1552,7 @@
         <v>72</v>
       </c>
       <c r="D7" t="s">
-        <v>72</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1478,7 +1566,7 @@
         <v>72</v>
       </c>
       <c r="D8" t="s">
-        <v>84</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1492,7 +1580,7 @@
         <v>72</v>
       </c>
       <c r="D9" t="s">
-        <v>92</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1506,7 +1594,7 @@
         <v>72</v>
       </c>
       <c r="D10" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1520,7 +1608,7 @@
         <v>72</v>
       </c>
       <c r="D11" t="s">
-        <v>89</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1534,7 +1622,7 @@
         <v>72</v>
       </c>
       <c r="D12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1548,7 +1636,7 @@
         <v>72</v>
       </c>
       <c r="D13" t="s">
-        <v>72</v>
+        <v>103</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1562,7 +1650,7 @@
         <v>72</v>
       </c>
       <c r="D14" t="s">
-        <v>72</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1576,7 +1664,7 @@
         <v>72</v>
       </c>
       <c r="D15" t="s">
-        <v>92</v>
+        <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1590,10 +1678,10 @@
         <v>72</v>
       </c>
       <c r="D16" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -1604,10 +1692,10 @@
         <v>72</v>
       </c>
       <c r="D17" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>54</v>
       </c>
@@ -1618,10 +1706,10 @@
         <v>72</v>
       </c>
       <c r="D18" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>55</v>
       </c>
@@ -1632,10 +1720,10 @@
         <v>72</v>
       </c>
       <c r="D19" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>56</v>
       </c>
@@ -1646,10 +1734,10 @@
         <v>72</v>
       </c>
       <c r="D20" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>57</v>
       </c>
@@ -1660,10 +1748,10 @@
         <v>72</v>
       </c>
       <c r="D21" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>58</v>
       </c>
@@ -1674,10 +1762,10 @@
         <v>72</v>
       </c>
       <c r="D22" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>59</v>
       </c>
@@ -1688,10 +1776,10 @@
         <v>72</v>
       </c>
       <c r="D23" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>60</v>
       </c>
@@ -1702,10 +1790,10 @@
         <v>72</v>
       </c>
       <c r="D24" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>61</v>
       </c>
@@ -1716,10 +1804,10 @@
         <v>72</v>
       </c>
       <c r="D25" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>62</v>
       </c>
@@ -1730,10 +1818,10 @@
         <v>72</v>
       </c>
       <c r="D26" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>63</v>
       </c>
@@ -1744,10 +1832,10 @@
         <v>72</v>
       </c>
       <c r="D27" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>64</v>
       </c>
@@ -1758,10 +1846,10 @@
         <v>72</v>
       </c>
       <c r="D28" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>65</v>
       </c>
@@ -1772,10 +1860,10 @@
         <v>72</v>
       </c>
       <c r="D29" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>66</v>
       </c>
@@ -1786,10 +1874,10 @@
         <v>72</v>
       </c>
       <c r="D30" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>67</v>
       </c>
@@ -1800,10 +1888,10 @@
         <v>72</v>
       </c>
       <c r="D31" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>68</v>
       </c>
@@ -1814,7 +1902,97 @@
         <v>72</v>
       </c>
       <c r="D32" t="s">
-        <v>89</v>
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="57.140625" collapsed="false"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>96</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>